<commit_message>
fix logic search unit berdasarkan lokasi dan jenis alat
</commit_message>
<xml_diff>
--- a/Benchmark_Per_HP_Alat_Berat.xlsx
+++ b/Benchmark_Per_HP_Alat_Berat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\SPIL\bbm\Analisa BBM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3728FF21-5760-4ACF-A43B-E286A417E1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515FD68E-6E13-4263-8B78-C62B33637EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit_Aktif" sheetId="1" r:id="rId1"/>
@@ -1394,7 +1394,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1453,7 +1453,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>23.57</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>2215.3000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>102.96</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>1187.72</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>96.34</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>47.71</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>10.37</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>4321.9399999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>897.89</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>787.02</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>830.24</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>966.23</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>98.71</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>53</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>53</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>161.99</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>53</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>5767</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>33</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>127</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>22</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>26</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>534.39</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>127</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>127</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>22</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>127</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>127</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>567.27</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>127</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>2942.11</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>127</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>127</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>127</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>3295.39</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>127</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>2154.1799999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>127</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>143</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>145</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>145</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>681.26</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>145</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>127</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>2727.68</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>127</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>127</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>127</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>47.97</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>153</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>4031.34</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>153</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>4994.53</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>156</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>158</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>156</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>527.29999999999995</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>156</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>22</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>22</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>22</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>22</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>22</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>464.52</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>22</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>2286.75</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>22</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>22</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>1845.29</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>22</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>22</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>486.98</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>22</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>22</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>22</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>1397.09</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>22</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>1790.06</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>153</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>22</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>165.99</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>153</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>22</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>2494.92</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>22</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>2278.2199999999998</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>22</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>22</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>1319.81</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>22</v>
       </c>
@@ -5899,7 +5899,7 @@
         <v>2425.4699999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>22</v>
       </c>
@@ -5937,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>22</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>22</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>641.13</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>22</v>
       </c>
@@ -6051,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>22</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>2505.06</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>22</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>22</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>3999.82</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>22</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>195.24</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>22</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>153</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>153</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>153</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>1181.4100000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>153</v>
       </c>
@@ -6393,7 +6393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>153</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>7813.63</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>153</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>22</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>22</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>2248.1</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>22</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>577.03</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>22</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>8655.17</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>22</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>127</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>127</v>
       </c>
@@ -6735,7 +6735,7 @@
         <v>1069.1400000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>22</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>22</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>16933.8</v>
       </c>
     </row>
-    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>211</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>1512.45</v>
       </c>
     </row>
-    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>33</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>119.67</v>
       </c>
     </row>
-    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>33</v>
       </c>
@@ -6963,7 +6963,7 @@
         <v>244.79</v>
       </c>
     </row>
-    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>53</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>795.67</v>
       </c>
     </row>
-    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>53</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>218</v>
       </c>
@@ -7077,7 +7077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>153</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>5972.93</v>
       </c>
     </row>
-    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>222</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>311.29000000000002</v>
       </c>
     </row>
-    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>224</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>30</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>1349.94</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>33</v>
       </c>
@@ -7267,7 +7267,7 @@
         <v>489.57</v>
       </c>
     </row>
-    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>53</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>2761.13</v>
       </c>
     </row>
-    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>218</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>5536.4</v>
       </c>
     </row>
-    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>127</v>
       </c>
@@ -7381,7 +7381,7 @@
         <v>2721.06</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>222</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>251.17</v>
       </c>
     </row>
-    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>17</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>1256.8699999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>12</v>
       </c>
@@ -7609,7 +7609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>33</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>17</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>127</v>
       </c>
@@ -7761,7 +7761,7 @@
         <v>1035.8900000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>53</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>222</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>33</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>12</v>
       </c>
@@ -8255,7 +8255,7 @@
         <v>28.58</v>
       </c>
     </row>
-    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>30</v>
       </c>
@@ -8331,7 +8331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>268</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>53</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>1182.4100000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>127</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>4265.5</v>
       </c>
     </row>
-    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>222</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>53</v>
       </c>
@@ -8521,7 +8521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>211</v>
       </c>
@@ -8563,8 +8563,7 @@
   <autoFilter ref="A1:L188" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="TRAILER"/>
-        <filter val="TRONTON"/>
+        <filter val="FORKLIFT"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -9299,10 +9298,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -9340,7 +9340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>4507</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -9386,7 +9386,7 @@
         <v>4248</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -9409,7 +9409,7 @@
         <v>3908</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -9432,7 +9432,7 @@
         <v>4463</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>4727</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -9478,7 +9478,7 @@
         <v>4489</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>4948</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>156</v>
       </c>
@@ -9524,7 +9524,7 @@
         <v>4420</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>156</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>4792</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -9593,7 +9593,7 @@
         <v>1072.3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -9616,7 +9616,7 @@
         <v>3665</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -9639,7 +9639,7 @@
         <v>2613</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -9662,7 +9662,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>3923</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>127</v>
       </c>
@@ -9708,7 +9708,7 @@
         <v>3795</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -9731,7 +9731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>127</v>
       </c>
@@ -9754,7 +9754,7 @@
         <v>3227</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -9777,7 +9777,7 @@
         <v>3901</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>127</v>
       </c>
@@ -9800,7 +9800,7 @@
         <v>2835</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -9823,7 +9823,7 @@
         <v>3565</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>127</v>
       </c>
@@ -9846,7 +9846,7 @@
         <v>2643</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>3387</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>127</v>
       </c>
@@ -9892,7 +9892,7 @@
         <v>4344</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>3789</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -9938,7 +9938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -9961,7 +9961,7 @@
         <v>2858</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>127</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>3485</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>127</v>
       </c>
@@ -10007,7 +10007,7 @@
         <v>4822</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>127</v>
       </c>
@@ -10030,7 +10030,7 @@
         <v>4364</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>156</v>
       </c>
@@ -10053,7 +10053,7 @@
         <v>5549</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>156</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>4840</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -10099,7 +10099,7 @@
         <v>3383</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>156</v>
       </c>
@@ -10122,7 +10122,7 @@
         <v>5566</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>156</v>
       </c>
@@ -10145,7 +10145,7 @@
         <v>4536</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -10168,7 +10168,7 @@
         <v>4154</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -10191,7 +10191,7 @@
         <v>2574</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -10214,7 +10214,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -10237,7 +10237,7 @@
         <v>4949</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -10260,7 +10260,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -10283,7 +10283,7 @@
         <v>4676</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>153</v>
       </c>
@@ -10306,7 +10306,7 @@
         <v>327.89999999999958</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -10329,7 +10329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>127</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>2964</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>127</v>
       </c>
@@ -10375,7 +10375,7 @@
         <v>3995</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -10467,7 +10467,7 @@
         <v>848.29999999999973</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>242</v>
       </c>
@@ -10490,7 +10490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>329</v>
       </c>
@@ -10560,7 +10560,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G54" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A1:G54" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="FORKLIFT"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>